<commit_message>
correction \times & excel
</commit_message>
<xml_diff>
--- a/PC2/Diff/DIFF/KCl/Differenz_Spline_Linear_KCl.xlsx
+++ b/PC2/Diff/DIFF/KCl/Differenz_Spline_Linear_KCl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49157\OneDrive\Desktop\Protokolle\PC2\Diff\DIFF\KCl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F34E8F-96DC-40C1-9D99-48E2982F46AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0703B3B-5052-4C28-851F-D656BA4E9728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D3D6A022-5070-4B86-8350-B65243CB1488}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2266,7 +2266,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2604,6 +2604,10 @@
         <f t="shared" si="2"/>
         <v>10698.022530915938</v>
       </c>
+      <c r="H12">
+        <f>H3/H2</f>
+        <v>2.6882711817114248E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">

</xml_diff>